<commit_message>
replacing unknowns and invalid category values as null
</commit_message>
<xml_diff>
--- a/DIAS Attributes - Values 2017.xlsx
+++ b/DIAS Attributes - Values 2017.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nareshsharma/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30532539-D3BC-CD44-80A3-400D1F31AC08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623CF29-4D56-A849-9B11-1F1975094333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="1226">
   <si>
     <t>AGER_TYP</t>
   </si>
@@ -3700,6 +3700,9 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Continuous</t>
   </si>
 </sst>
 </file>
@@ -4433,8 +4436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F2260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4442,7 +4445,7 @@
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" customWidth="1"/>
     <col min="3" max="3" width="53.5" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="76.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4865,7 +4868,7 @@
         <v>872</v>
       </c>
       <c r="F39" s="57" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4882,7 +4885,7 @@
         <v>872</v>
       </c>
       <c r="F40" s="57" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4899,7 +4902,7 @@
         <v>873</v>
       </c>
       <c r="F41" s="57" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4916,7 +4919,7 @@
         <v>872</v>
       </c>
       <c r="F42" s="57" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
@@ -12251,8 +12254,8 @@
       <c r="E714" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="F714" s="57" t="s">
-        <v>1223</v>
+      <c r="F714" s="60" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="715" spans="2:6" ht="16" x14ac:dyDescent="0.2">
@@ -17352,8 +17355,8 @@
       <c r="E1170" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="F1170" s="57" t="s">
-        <v>1223</v>
+      <c r="F1170" s="60" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="1171" spans="2:6" x14ac:dyDescent="0.2">
@@ -26304,8 +26307,8 @@
       <c r="E1989" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="F1989" t="s">
-        <v>1223</v>
+      <c r="F1989" s="60" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="1990" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
customers and general data shape matching
</commit_message>
<xml_diff>
--- a/DIAS Attributes - Values 2017.xlsx
+++ b/DIAS Attributes - Values 2017.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nareshsharma/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nareshsharma/Documents/repos/udacity-capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623CF29-4D56-A849-9B11-1F1975094333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB038DB-F3EB-A948-9C8C-CA1F55344A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="1225">
   <si>
     <t>AGER_TYP</t>
   </si>
@@ -3700,9 +3700,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Continuous</t>
   </si>
 </sst>
 </file>
@@ -4077,6 +4074,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4092,10 +4093,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4436,8 +4433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F2260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A1973" workbookViewId="0">
+      <selection activeCell="G1992" sqref="G1992"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4479,7 +4476,7 @@
       <c r="E3" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -4536,7 +4533,7 @@
       <c r="E8" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -4603,7 +4600,7 @@
       <c r="E14" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -4830,7 +4827,7 @@
       <c r="E36" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F36" s="57" t="s">
+      <c r="F36" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -4867,8 +4864,8 @@
       <c r="E39" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="F39" s="57" t="s">
-        <v>1225</v>
+      <c r="F39" s="52" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4884,8 +4881,8 @@
       <c r="E40" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="F40" s="57" t="s">
-        <v>1225</v>
+      <c r="F40" s="52" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4901,8 +4898,8 @@
       <c r="E41" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="F41" s="57" t="s">
-        <v>1225</v>
+      <c r="F41" s="52" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4918,8 +4915,8 @@
       <c r="E42" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="F42" s="57" t="s">
-        <v>1225</v>
+      <c r="F42" s="52" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
@@ -4935,7 +4932,7 @@
       <c r="E43" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F43" s="57" t="s">
+      <c r="F43" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -5022,7 +5019,7 @@
       <c r="E51" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F51" s="57" t="s">
+      <c r="F51" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -5059,7 +5056,7 @@
       <c r="E54" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F54" s="57" t="s">
+      <c r="F54" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -5166,7 +5163,7 @@
       <c r="E64" s="5" t="s">
         <v>1085</v>
       </c>
-      <c r="F64" s="57" t="s">
+      <c r="F64" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -5613,7 +5610,7 @@
       <c r="E108" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F108" s="57" t="s">
+      <c r="F108" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -5882,7 +5879,7 @@
       <c r="E134" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F134" s="57" t="s">
+      <c r="F134" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -5959,7 +5956,7 @@
       <c r="E141" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F141" s="57" t="s">
+      <c r="F141" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -6036,7 +6033,7 @@
       <c r="E148" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F148" s="57" t="s">
+      <c r="F148" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -6113,7 +6110,7 @@
       <c r="E155" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F155" s="57" t="s">
+      <c r="F155" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6220,7 +6217,7 @@
       <c r="E165" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F165" s="57" t="s">
+      <c r="F165" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6309,7 +6306,7 @@
       <c r="E173" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F173" s="57" t="s">
+      <c r="F173" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6398,7 +6395,7 @@
       <c r="E181" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F181" s="57" t="s">
+      <c r="F181" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6487,7 +6484,7 @@
       <c r="E189" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F189" s="57" t="s">
+      <c r="F189" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6594,7 +6591,7 @@
       <c r="E199" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F199" s="57" t="s">
+      <c r="F199" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6701,7 +6698,7 @@
       <c r="E209" s="5" t="s">
         <v>795</v>
       </c>
-      <c r="F209" s="57" t="s">
+      <c r="F209" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -6818,7 +6815,7 @@
       <c r="E220" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F220" s="57" t="s">
+      <c r="F220" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6907,7 +6904,7 @@
       <c r="E228" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F228" s="57" t="s">
+      <c r="F228" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -6996,7 +6993,7 @@
       <c r="E236" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F236" s="57" t="s">
+      <c r="F236" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7085,7 +7082,7 @@
       <c r="E244" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F244" s="57" t="s">
+      <c r="F244" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7174,7 +7171,7 @@
       <c r="E252" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F252" s="57" t="s">
+      <c r="F252" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7263,7 +7260,7 @@
       <c r="E260" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F260" s="57" t="s">
+      <c r="F260" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7352,7 +7349,7 @@
       <c r="E268" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F268" s="57" t="s">
+      <c r="F268" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7441,7 +7438,7 @@
       <c r="E276" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F276" s="57" t="s">
+      <c r="F276" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7530,7 +7527,7 @@
       <c r="E284" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F284" s="57" t="s">
+      <c r="F284" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7619,7 +7616,7 @@
       <c r="E292" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F292" s="57" t="s">
+      <c r="F292" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7708,7 +7705,7 @@
       <c r="E300" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F300" s="57" t="s">
+      <c r="F300" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -7797,7 +7794,7 @@
       <c r="E308" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F308" s="57" t="s">
+      <c r="F308" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -7874,7 +7871,7 @@
       <c r="E315" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F315" s="57" t="s">
+      <c r="F315" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -7951,7 +7948,7 @@
       <c r="E322" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F322" s="57" t="s">
+      <c r="F322" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8058,7 +8055,7 @@
       <c r="E332" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="F332" s="58" t="s">
+      <c r="F332" s="53" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8165,7 +8162,7 @@
       <c r="E342" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="F342" s="58" t="s">
+      <c r="F342" s="53" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8272,7 +8269,7 @@
       <c r="E352" s="50" t="s">
         <v>795</v>
       </c>
-      <c r="F352" s="58" t="s">
+      <c r="F352" s="53" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -8389,7 +8386,7 @@
       <c r="E363" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F363" s="57" t="s">
+      <c r="F363" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8478,7 +8475,7 @@
       <c r="E371" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F371" s="57" t="s">
+      <c r="F371" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8567,7 +8564,7 @@
       <c r="E379" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F379" s="57" t="s">
+      <c r="F379" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8656,7 +8653,7 @@
       <c r="E387" s="2" t="s">
         <v>1168</v>
       </c>
-      <c r="F387" s="57" t="s">
+      <c r="F387" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8733,7 +8730,7 @@
       <c r="E394" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F394" s="57" t="s">
+      <c r="F394" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8810,7 +8807,7 @@
       <c r="E401" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F401" s="57" t="s">
+      <c r="F401" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8899,7 +8896,7 @@
       <c r="E409" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F409" s="57" t="s">
+      <c r="F409" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -8988,7 +8985,7 @@
       <c r="E417" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F417" s="57" t="s">
+      <c r="F417" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9077,7 +9074,7 @@
       <c r="E425" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F425" s="57" t="s">
+      <c r="F425" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9166,7 +9163,7 @@
       <c r="E433" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F433" s="57" t="s">
+      <c r="F433" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9255,7 +9252,7 @@
       <c r="E441" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F441" s="57" t="s">
+      <c r="F441" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9344,7 +9341,7 @@
       <c r="E449" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F449" s="57" t="s">
+      <c r="F449" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9433,7 +9430,7 @@
       <c r="E457" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F457" s="57" t="s">
+      <c r="F457" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9522,7 +9519,7 @@
       <c r="E465" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F465" s="57" t="s">
+      <c r="F465" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9611,7 +9608,7 @@
       <c r="E473" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F473" s="57" t="s">
+      <c r="F473" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9700,7 +9697,7 @@
       <c r="E481" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F481" s="57" t="s">
+      <c r="F481" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9777,7 +9774,7 @@
       <c r="E488" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F488" s="57" t="s">
+      <c r="F488" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9854,7 +9851,7 @@
       <c r="E495" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F495" s="57" t="s">
+      <c r="F495" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -9961,7 +9958,7 @@
       <c r="E505" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F505" s="57" t="s">
+      <c r="F505" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10050,7 +10047,7 @@
       <c r="E513" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F513" s="57" t="s">
+      <c r="F513" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10157,7 +10154,7 @@
       <c r="E523" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F523" s="57" t="s">
+      <c r="F523" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10264,7 +10261,7 @@
       <c r="E533" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F533" s="57" t="s">
+      <c r="F533" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10353,7 +10350,7 @@
       <c r="E541" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F541" s="57" t="s">
+      <c r="F541" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10442,7 +10439,7 @@
       <c r="E549" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F549" s="57" t="s">
+      <c r="F549" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -10519,7 +10516,7 @@
       <c r="E556" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F556" s="57" t="s">
+      <c r="F556" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -10596,7 +10593,7 @@
       <c r="E563" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F563" s="57" t="s">
+      <c r="F563" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10703,7 +10700,7 @@
       <c r="E573" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F573" s="57" t="s">
+      <c r="F573" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10810,7 +10807,7 @@
       <c r="E583" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F583" s="57" t="s">
+      <c r="F583" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10917,7 +10914,7 @@
       <c r="E593" s="5" t="s">
         <v>795</v>
       </c>
-      <c r="F593" s="57" t="s">
+      <c r="F593" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11034,7 +11031,7 @@
       <c r="E604" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F604" s="57" t="s">
+      <c r="F604" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -11123,7 +11120,7 @@
       <c r="E612" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F612" s="57" t="s">
+      <c r="F612" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -11212,7 +11209,7 @@
       <c r="E620" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F620" s="57" t="s">
+      <c r="F620" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11289,7 +11286,7 @@
       <c r="E627" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F627" s="57" t="s">
+      <c r="F627" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11366,7 +11363,7 @@
       <c r="E634" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F634" s="57" t="s">
+      <c r="F634" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -11455,7 +11452,7 @@
       <c r="E642" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F642" s="57" t="s">
+      <c r="F642" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -11544,7 +11541,7 @@
       <c r="E650" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F650" s="57" t="s">
+      <c r="F650" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11621,7 +11618,7 @@
       <c r="E657" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F657" s="57" t="s">
+      <c r="F657" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -11698,7 +11695,7 @@
       <c r="E664" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F664" s="57" t="s">
+      <c r="F664" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11765,7 +11762,7 @@
       <c r="E670" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F670" s="57" t="s">
+      <c r="F670" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11832,7 +11829,7 @@
       <c r="E676" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F676" s="57" t="s">
+      <c r="F676" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11899,7 +11896,7 @@
       <c r="E682" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F682" s="57" t="s">
+      <c r="F682" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -11966,7 +11963,7 @@
       <c r="E688" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F688" s="57" t="s">
+      <c r="F688" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -12033,7 +12030,7 @@
       <c r="E694" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F694" s="57" t="s">
+      <c r="F694" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -12100,7 +12097,7 @@
       <c r="E700" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F700" s="57" t="s">
+      <c r="F700" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -12197,7 +12194,7 @@
       <c r="E709" s="2" t="s">
         <v>1079</v>
       </c>
-      <c r="F709" s="57" t="s">
+      <c r="F709" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -12254,8 +12251,8 @@
       <c r="E714" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="F714" s="60" t="s">
-        <v>1225</v>
+      <c r="F714" s="55" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="715" spans="2:6" ht="16" x14ac:dyDescent="0.2">
@@ -12271,7 +12268,7 @@
       <c r="E715" s="28" t="s">
         <v>1156</v>
       </c>
-      <c r="F715" s="57" t="s">
+      <c r="F715" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -12398,7 +12395,7 @@
       <c r="E727" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F727" s="57" t="s">
+      <c r="F727" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -12485,7 +12482,7 @@
       <c r="E735" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="F735" s="57" t="s">
+      <c r="F735" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -12514,7 +12511,7 @@
       <c r="E737" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F737" s="57" t="s">
+      <c r="F737" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -12621,7 +12618,7 @@
       <c r="E747" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F747" s="57" t="s">
+      <c r="F747" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -12678,7 +12675,7 @@
       <c r="E752" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F752" s="57" t="s">
+      <c r="F752" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -12755,7 +12752,7 @@
       <c r="E759" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F759" s="57" t="s">
+      <c r="F759" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -12852,7 +12849,7 @@
       <c r="E768" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F768" s="57" t="s">
+      <c r="F768" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -12919,7 +12916,7 @@
       <c r="E774" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F774" s="57" t="s">
+      <c r="F774" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -12986,7 +12983,7 @@
       <c r="E780" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F780" s="57" t="s">
+      <c r="F780" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13053,7 +13050,7 @@
       <c r="E786" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F786" s="57" t="s">
+      <c r="F786" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13130,7 +13127,7 @@
       <c r="E793" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F793" s="57" t="s">
+      <c r="F793" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13187,7 +13184,7 @@
       <c r="E798" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F798" s="57" t="s">
+      <c r="F798" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13254,7 +13251,7 @@
       <c r="E804" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F804" s="57" t="s">
+      <c r="F804" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13321,7 +13318,7 @@
       <c r="E810" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F810" s="57" t="s">
+      <c r="F810" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13378,7 +13375,7 @@
       <c r="E815" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F815" s="57" t="s">
+      <c r="F815" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13425,7 +13422,7 @@
       <c r="E819" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="F819" s="57" t="s">
+      <c r="F819" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13492,7 +13489,7 @@
       <c r="E825" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F825" s="57" t="s">
+      <c r="F825" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13559,7 +13556,7 @@
       <c r="E831" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F831" s="57" t="s">
+      <c r="F831" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13626,7 +13623,7 @@
       <c r="E837" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F837" s="57" t="s">
+      <c r="F837" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13693,7 +13690,7 @@
       <c r="E843" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F843" s="57" t="s">
+      <c r="F843" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13760,7 +13757,7 @@
       <c r="E849" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F849" s="57" t="s">
+      <c r="F849" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13827,7 +13824,7 @@
       <c r="E855" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F855" s="57" t="s">
+      <c r="F855" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13894,7 +13891,7 @@
       <c r="E861" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F861" s="57" t="s">
+      <c r="F861" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -13961,7 +13958,7 @@
       <c r="E867" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F867" s="57" t="s">
+      <c r="F867" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14028,7 +14025,7 @@
       <c r="E873" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F873" s="57" t="s">
+      <c r="F873" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14105,7 +14102,7 @@
       <c r="E880" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F880" s="57" t="s">
+      <c r="F880" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14182,7 +14179,7 @@
       <c r="E887" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F887" s="57" t="s">
+      <c r="F887" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14259,7 +14256,7 @@
       <c r="E894" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F894" s="57" t="s">
+      <c r="F894" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14336,7 +14333,7 @@
       <c r="E901" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F901" s="57" t="s">
+      <c r="F901" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14413,7 +14410,7 @@
       <c r="E908" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F908" s="57" t="s">
+      <c r="F908" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14480,7 +14477,7 @@
       <c r="E914" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F914" s="57" t="s">
+      <c r="F914" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14547,7 +14544,7 @@
       <c r="E920" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F920" s="57" t="s">
+      <c r="F920" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14614,7 +14611,7 @@
       <c r="E926" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F926" s="57" t="s">
+      <c r="F926" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14681,7 +14678,7 @@
       <c r="E932" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F932" s="57" t="s">
+      <c r="F932" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14748,7 +14745,7 @@
       <c r="E938" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F938" s="57" t="s">
+      <c r="F938" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14795,7 +14792,7 @@
       <c r="E942" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F942" s="57" t="s">
+      <c r="F942" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14842,7 +14839,7 @@
       <c r="E946" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F946" s="57" t="s">
+      <c r="F946" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14889,7 +14886,7 @@
       <c r="E950" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F950" s="57" t="s">
+      <c r="F950" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -14936,7 +14933,7 @@
       <c r="E954" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F954" s="57" t="s">
+      <c r="F954" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15003,7 +15000,7 @@
       <c r="E960" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F960" s="57" t="s">
+      <c r="F960" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15070,7 +15067,7 @@
       <c r="E966" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F966" s="57" t="s">
+      <c r="F966" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15137,7 +15134,7 @@
       <c r="E972" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F972" s="57" t="s">
+      <c r="F972" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15204,7 +15201,7 @@
       <c r="E978" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F978" s="57" t="s">
+      <c r="F978" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15261,7 +15258,7 @@
       <c r="E983" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F983" s="57" t="s">
+      <c r="F983" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -15328,7 +15325,7 @@
       <c r="E989" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F989" s="57" t="s">
+      <c r="F989" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -15385,7 +15382,7 @@
       <c r="E994" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F994" s="57" t="s">
+      <c r="F994" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -15432,7 +15429,7 @@
       <c r="E998" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F998" s="57" t="s">
+      <c r="F998" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15499,7 +15496,7 @@
       <c r="E1004" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1004" s="57" t="s">
+      <c r="F1004" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15566,7 +15563,7 @@
       <c r="E1010" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1010" s="57" t="s">
+      <c r="F1010" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15633,7 +15630,7 @@
       <c r="E1016" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1016" s="57" t="s">
+      <c r="F1016" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15710,7 +15707,7 @@
       <c r="E1023" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1023" s="57" t="s">
+      <c r="F1023" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15767,7 +15764,7 @@
       <c r="E1028" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1028" s="57" t="s">
+      <c r="F1028" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -15834,7 +15831,7 @@
       <c r="E1034" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1034" s="57" t="s">
+      <c r="F1034" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -15891,7 +15888,7 @@
       <c r="E1039" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1039" s="57" t="s">
+      <c r="F1039" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -15948,7 +15945,7 @@
       <c r="E1044" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1044" s="57" t="s">
+      <c r="F1044" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16005,7 +16002,7 @@
       <c r="E1049" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1049" s="57" t="s">
+      <c r="F1049" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16072,7 +16069,7 @@
       <c r="E1055" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1055" s="57" t="s">
+      <c r="F1055" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16139,7 +16136,7 @@
       <c r="E1061" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1061" s="57" t="s">
+      <c r="F1061" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16206,7 +16203,7 @@
       <c r="E1067" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1067" s="57" t="s">
+      <c r="F1067" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16273,7 +16270,7 @@
       <c r="E1073" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1073" s="57" t="s">
+      <c r="F1073" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16340,7 +16337,7 @@
       <c r="E1079" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1079" s="57" t="s">
+      <c r="F1079" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16377,7 +16374,7 @@
       <c r="E1082" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1082" s="57" t="s">
+      <c r="F1082" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16434,7 +16431,7 @@
       <c r="E1087" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1087" s="57" t="s">
+      <c r="F1087" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16491,7 +16488,7 @@
       <c r="E1092" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1092" s="57" t="s">
+      <c r="F1092" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16548,7 +16545,7 @@
       <c r="E1097" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1097" s="57" t="s">
+      <c r="F1097" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16615,7 +16612,7 @@
       <c r="E1103" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1103" s="57" t="s">
+      <c r="F1103" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16682,7 +16679,7 @@
       <c r="E1109" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1109" s="57" t="s">
+      <c r="F1109" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16759,7 +16756,7 @@
       <c r="E1116" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1116" s="57" t="s">
+      <c r="F1116" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16826,7 +16823,7 @@
       <c r="E1122" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1122" s="57" t="s">
+      <c r="F1122" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16893,7 +16890,7 @@
       <c r="E1128" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1128" s="57" t="s">
+      <c r="F1128" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16970,7 +16967,7 @@
       <c r="E1135" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="F1135" s="57" t="s">
+      <c r="F1135" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17047,7 +17044,7 @@
       <c r="E1142" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1142" s="57" t="s">
+      <c r="F1142" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17124,7 +17121,7 @@
       <c r="E1149" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1149" s="57" t="s">
+      <c r="F1149" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17201,7 +17198,7 @@
       <c r="E1156" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1156" s="57" t="s">
+      <c r="F1156" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17278,7 +17275,7 @@
       <c r="E1163" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1163" s="57" t="s">
+      <c r="F1163" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17355,8 +17352,8 @@
       <c r="E1170" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="F1170" s="60" t="s">
-        <v>1225</v>
+      <c r="F1170" s="55" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="1171" spans="2:6" x14ac:dyDescent="0.2">
@@ -17372,7 +17369,7 @@
       <c r="E1171" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1171" s="57" t="s">
+      <c r="F1171" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17449,7 +17446,7 @@
       <c r="E1178" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1178" s="57" t="s">
+      <c r="F1178" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17526,7 +17523,7 @@
       <c r="E1185" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1185" s="57" t="s">
+      <c r="F1185" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17603,7 +17600,7 @@
       <c r="E1192" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1192" s="57" t="s">
+      <c r="F1192" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17680,7 +17677,7 @@
       <c r="E1199" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1199" s="57" t="s">
+      <c r="F1199" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17757,7 +17754,7 @@
       <c r="E1206" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1206" s="57" t="s">
+      <c r="F1206" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17834,7 +17831,7 @@
       <c r="E1213" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1213" s="57" t="s">
+      <c r="F1213" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17911,7 +17908,7 @@
       <c r="E1220" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1220" s="57" t="s">
+      <c r="F1220" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -17988,7 +17985,7 @@
       <c r="E1227" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1227" s="57" t="s">
+      <c r="F1227" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18065,7 +18062,7 @@
       <c r="E1234" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1234" s="57" t="s">
+      <c r="F1234" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18142,7 +18139,7 @@
       <c r="E1241" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1241" s="57" t="s">
+      <c r="F1241" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18219,7 +18216,7 @@
       <c r="E1248" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1248" s="57" t="s">
+      <c r="F1248" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18296,7 +18293,7 @@
       <c r="E1255" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1255" s="57" t="s">
+      <c r="F1255" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18373,7 +18370,7 @@
       <c r="E1262" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1262" s="57" t="s">
+      <c r="F1262" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18450,7 +18447,7 @@
       <c r="E1269" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1269" s="57" t="s">
+      <c r="F1269" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18527,7 +18524,7 @@
       <c r="E1276" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1276" s="57" t="s">
+      <c r="F1276" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18604,7 +18601,7 @@
       <c r="E1283" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1283" s="57" t="s">
+      <c r="F1283" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18681,7 +18678,7 @@
       <c r="E1290" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1290" s="57" t="s">
+      <c r="F1290" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18758,7 +18755,7 @@
       <c r="E1297" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1297" s="57" t="s">
+      <c r="F1297" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18835,7 +18832,7 @@
       <c r="E1304" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1304" s="57" t="s">
+      <c r="F1304" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18912,7 +18909,7 @@
       <c r="E1311" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1311" s="57" t="s">
+      <c r="F1311" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -18989,7 +18986,7 @@
       <c r="E1318" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1318" s="57" t="s">
+      <c r="F1318" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19066,7 +19063,7 @@
       <c r="E1325" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1325" s="57" t="s">
+      <c r="F1325" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19143,7 +19140,7 @@
       <c r="E1332" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1332" s="57" t="s">
+      <c r="F1332" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19220,7 +19217,7 @@
       <c r="E1339" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1339" s="57" t="s">
+      <c r="F1339" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19297,7 +19294,7 @@
       <c r="E1346" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1346" s="57" t="s">
+      <c r="F1346" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19374,7 +19371,7 @@
       <c r="E1353" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1353" s="57" t="s">
+      <c r="F1353" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19451,7 +19448,7 @@
       <c r="E1360" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1360" s="57" t="s">
+      <c r="F1360" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19528,7 +19525,7 @@
       <c r="E1367" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1367" s="57" t="s">
+      <c r="F1367" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19605,7 +19602,7 @@
       <c r="E1374" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1374" s="57" t="s">
+      <c r="F1374" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19682,7 +19679,7 @@
       <c r="E1381" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1381" s="57" t="s">
+      <c r="F1381" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19759,7 +19756,7 @@
       <c r="E1388" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1388" s="57" t="s">
+      <c r="F1388" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19836,7 +19833,7 @@
       <c r="E1395" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1395" s="57" t="s">
+      <c r="F1395" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19913,7 +19910,7 @@
       <c r="E1402" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1402" s="57" t="s">
+      <c r="F1402" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -19990,7 +19987,7 @@
       <c r="E1409" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1409" s="57" t="s">
+      <c r="F1409" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20067,7 +20064,7 @@
       <c r="E1416" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1416" s="57" t="s">
+      <c r="F1416" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20144,7 +20141,7 @@
       <c r="E1423" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1423" s="57" t="s">
+      <c r="F1423" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20221,7 +20218,7 @@
       <c r="E1430" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1430" s="57" t="s">
+      <c r="F1430" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20298,7 +20295,7 @@
       <c r="E1437" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1437" s="57" t="s">
+      <c r="F1437" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20375,7 +20372,7 @@
       <c r="E1444" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1444" s="57" t="s">
+      <c r="F1444" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20452,7 +20449,7 @@
       <c r="E1451" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1451" s="57" t="s">
+      <c r="F1451" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20529,7 +20526,7 @@
       <c r="E1458" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1458" s="57" t="s">
+      <c r="F1458" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20606,7 +20603,7 @@
       <c r="E1465" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1465" s="57" t="s">
+      <c r="F1465" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20683,7 +20680,7 @@
       <c r="E1472" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1472" s="57" t="s">
+      <c r="F1472" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20760,7 +20757,7 @@
       <c r="E1479" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1479" s="57" t="s">
+      <c r="F1479" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20837,7 +20834,7 @@
       <c r="E1486" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1486" s="57" t="s">
+      <c r="F1486" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20914,7 +20911,7 @@
       <c r="E1493" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1493" s="57" t="s">
+      <c r="F1493" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -20991,7 +20988,7 @@
       <c r="E1500" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1500" s="57" t="s">
+      <c r="F1500" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21068,7 +21065,7 @@
       <c r="E1507" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1507" s="57" t="s">
+      <c r="F1507" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21145,7 +21142,7 @@
       <c r="E1514" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1514" s="57" t="s">
+      <c r="F1514" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21222,7 +21219,7 @@
       <c r="E1521" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1521" s="57" t="s">
+      <c r="F1521" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21299,7 +21296,7 @@
       <c r="E1528" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1528" s="57" t="s">
+      <c r="F1528" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21376,7 +21373,7 @@
       <c r="E1535" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1535" s="57" t="s">
+      <c r="F1535" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21453,7 +21450,7 @@
       <c r="E1542" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1542" s="57" t="s">
+      <c r="F1542" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21530,7 +21527,7 @@
       <c r="E1549" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1549" s="57" t="s">
+      <c r="F1549" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21607,7 +21604,7 @@
       <c r="E1556" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1556" s="57" t="s">
+      <c r="F1556" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21664,7 +21661,7 @@
       <c r="E1561" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1561" s="57" t="s">
+      <c r="F1561" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21721,7 +21718,7 @@
       <c r="E1566" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1566" s="57" t="s">
+      <c r="F1566" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21778,7 +21775,7 @@
       <c r="E1571" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1571" s="57" t="s">
+      <c r="F1571" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21835,7 +21832,7 @@
       <c r="E1576" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1576" s="57" t="s">
+      <c r="F1576" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21912,7 +21909,7 @@
       <c r="E1583" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1583" s="57" t="s">
+      <c r="F1583" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -21989,7 +21986,7 @@
       <c r="E1590" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1590" s="57" t="s">
+      <c r="F1590" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22066,7 +22063,7 @@
       <c r="E1597" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1597" s="57" t="s">
+      <c r="F1597" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22143,7 +22140,7 @@
       <c r="E1604" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1604" s="57" t="s">
+      <c r="F1604" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22220,7 +22217,7 @@
       <c r="E1611" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1611" s="57" t="s">
+      <c r="F1611" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22297,7 +22294,7 @@
       <c r="E1618" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1618" s="57" t="s">
+      <c r="F1618" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22374,7 +22371,7 @@
       <c r="E1625" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1625" s="57" t="s">
+      <c r="F1625" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22451,7 +22448,7 @@
       <c r="E1632" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1632" s="57" t="s">
+      <c r="F1632" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22528,7 +22525,7 @@
       <c r="E1639" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1639" s="57" t="s">
+      <c r="F1639" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22605,7 +22602,7 @@
       <c r="E1646" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1646" s="57" t="s">
+      <c r="F1646" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22682,7 +22679,7 @@
       <c r="E1653" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1653" s="57" t="s">
+      <c r="F1653" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22759,7 +22756,7 @@
       <c r="E1660" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1660" s="57" t="s">
+      <c r="F1660" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22836,7 +22833,7 @@
       <c r="E1667" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1667" s="57" t="s">
+      <c r="F1667" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22913,7 +22910,7 @@
       <c r="E1674" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1674" s="57" t="s">
+      <c r="F1674" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -22980,7 +22977,7 @@
       <c r="E1680" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1680" s="57" t="s">
+      <c r="F1680" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23057,7 +23054,7 @@
       <c r="E1687" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1687" s="57" t="s">
+      <c r="F1687" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23134,7 +23131,7 @@
       <c r="E1694" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1694" s="57" t="s">
+      <c r="F1694" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23211,7 +23208,7 @@
       <c r="E1701" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1701" s="57" t="s">
+      <c r="F1701" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23288,7 +23285,7 @@
       <c r="E1708" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1708" s="57" t="s">
+      <c r="F1708" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23365,7 +23362,7 @@
       <c r="E1715" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1715" s="57" t="s">
+      <c r="F1715" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23442,7 +23439,7 @@
       <c r="E1722" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1722" s="57" t="s">
+      <c r="F1722" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23519,7 +23516,7 @@
       <c r="E1729" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1729" s="57" t="s">
+      <c r="F1729" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23596,7 +23593,7 @@
       <c r="E1736" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1736" s="57" t="s">
+      <c r="F1736" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23673,7 +23670,7 @@
       <c r="E1743" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1743" s="57" t="s">
+      <c r="F1743" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23750,7 +23747,7 @@
       <c r="E1750" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1750" s="57" t="s">
+      <c r="F1750" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23827,7 +23824,7 @@
       <c r="E1757" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1757" s="57" t="s">
+      <c r="F1757" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23904,7 +23901,7 @@
       <c r="E1764" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1764" s="57" t="s">
+      <c r="F1764" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -23981,7 +23978,7 @@
       <c r="E1771" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1771" s="57" t="s">
+      <c r="F1771" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24058,7 +24055,7 @@
       <c r="E1778" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1778" s="57" t="s">
+      <c r="F1778" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24135,7 +24132,7 @@
       <c r="E1785" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1785" s="57" t="s">
+      <c r="F1785" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24212,7 +24209,7 @@
       <c r="E1792" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1792" s="57" t="s">
+      <c r="F1792" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24289,7 +24286,7 @@
       <c r="E1799" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1799" s="57" t="s">
+      <c r="F1799" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24366,7 +24363,7 @@
       <c r="E1806" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1806" s="57" t="s">
+      <c r="F1806" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24443,7 +24440,7 @@
       <c r="E1813" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1813" s="57" t="s">
+      <c r="F1813" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24520,7 +24517,7 @@
       <c r="E1820" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1820" s="57" t="s">
+      <c r="F1820" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24597,7 +24594,7 @@
       <c r="E1827" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1827" s="57" t="s">
+      <c r="F1827" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24674,7 +24671,7 @@
       <c r="E1834" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1834" s="57" t="s">
+      <c r="F1834" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24751,7 +24748,7 @@
       <c r="E1841" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1841" s="57" t="s">
+      <c r="F1841" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24828,7 +24825,7 @@
       <c r="E1848" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1848" s="57" t="s">
+      <c r="F1848" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24905,7 +24902,7 @@
       <c r="E1855" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F1855" s="57" t="s">
+      <c r="F1855" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -24982,7 +24979,7 @@
       <c r="E1862" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1862" s="57" t="s">
+      <c r="F1862" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -25059,7 +25056,7 @@
       <c r="E1869" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F1869" s="57" t="s">
+      <c r="F1869" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -25136,7 +25133,7 @@
       <c r="E1876" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F1876" s="57" t="s">
+      <c r="F1876" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -25213,7 +25210,7 @@
       <c r="E1883" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1883" s="57" t="s">
+      <c r="F1883" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -25270,7 +25267,7 @@
       <c r="E1888" s="2" t="s">
         <v>1055</v>
       </c>
-      <c r="F1888" s="57" t="s">
+      <c r="F1888" s="52" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -25347,7 +25344,7 @@
       <c r="E1895" s="2" t="s">
         <v>993</v>
       </c>
-      <c r="F1895" s="57" t="s">
+      <c r="F1895" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -25464,7 +25461,7 @@
       <c r="E1906" s="2" t="s">
         <v>993</v>
       </c>
-      <c r="F1906" s="60" t="s">
+      <c r="F1906" s="55" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -25484,7 +25481,7 @@
       <c r="D1908" s="19">
         <v>3</v>
       </c>
-      <c r="E1908" s="52" t="s">
+      <c r="E1908" s="56" t="s">
         <v>1017</v>
       </c>
     </row>
@@ -25494,7 +25491,7 @@
       <c r="D1909" s="7">
         <v>4</v>
       </c>
-      <c r="E1909" s="54"/>
+      <c r="E1909" s="58"/>
     </row>
     <row r="1910" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1910" s="34"/>
@@ -25502,7 +25499,7 @@
       <c r="D1910" s="20">
         <v>5</v>
       </c>
-      <c r="E1910" s="53"/>
+      <c r="E1910" s="57"/>
     </row>
     <row r="1911" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1911" s="34"/>
@@ -25510,7 +25507,7 @@
       <c r="D1911" s="19">
         <v>6</v>
       </c>
-      <c r="E1911" s="52" t="s">
+      <c r="E1911" s="56" t="s">
         <v>1018</v>
       </c>
     </row>
@@ -25520,7 +25517,7 @@
       <c r="D1912" s="7">
         <v>7</v>
       </c>
-      <c r="E1912" s="54"/>
+      <c r="E1912" s="58"/>
     </row>
     <row r="1913" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1913" s="34"/>
@@ -25528,7 +25525,7 @@
       <c r="D1913" s="20">
         <v>8</v>
       </c>
-      <c r="E1913" s="53"/>
+      <c r="E1913" s="57"/>
     </row>
     <row r="1914" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1914" s="34"/>
@@ -25536,7 +25533,7 @@
       <c r="D1914" s="7">
         <v>9</v>
       </c>
-      <c r="E1914" s="52" t="s">
+      <c r="E1914" s="56" t="s">
         <v>1019</v>
       </c>
     </row>
@@ -25546,7 +25543,7 @@
       <c r="D1915" s="7">
         <v>10</v>
       </c>
-      <c r="E1915" s="54"/>
+      <c r="E1915" s="58"/>
     </row>
     <row r="1916" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1916" s="34"/>
@@ -25554,7 +25551,7 @@
       <c r="D1916" s="7">
         <v>11</v>
       </c>
-      <c r="E1916" s="55"/>
+      <c r="E1916" s="59"/>
     </row>
     <row r="1917" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1917" s="33" t="s">
@@ -25569,7 +25566,7 @@
       <c r="E1917" s="5" t="s">
         <v>971</v>
       </c>
-      <c r="F1917" s="57" t="s">
+      <c r="F1917" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -25976,7 +25973,7 @@
       <c r="E1957" s="2" t="s">
         <v>992</v>
       </c>
-      <c r="F1957" s="57" t="s">
+      <c r="F1957" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -26103,7 +26100,7 @@
       <c r="E1969" s="5" t="s">
         <v>1021</v>
       </c>
-      <c r="F1969" s="57" t="s">
+      <c r="F1969" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -26207,7 +26204,7 @@
       <c r="D1979" s="4">
         <v>1</v>
       </c>
-      <c r="E1979" s="56" t="s">
+      <c r="E1979" s="60" t="s">
         <v>1034</v>
       </c>
       <c r="F1979" t="s">
@@ -26220,7 +26217,7 @@
       <c r="D1980" s="20">
         <v>2</v>
       </c>
-      <c r="E1980" s="53"/>
+      <c r="E1980" s="57"/>
     </row>
     <row r="1981" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1981" s="36"/>
@@ -26228,7 +26225,7 @@
       <c r="D1981" s="19">
         <v>3</v>
       </c>
-      <c r="E1981" s="52" t="s">
+      <c r="E1981" s="56" t="s">
         <v>1035</v>
       </c>
     </row>
@@ -26238,7 +26235,7 @@
       <c r="D1982" s="7">
         <v>4</v>
       </c>
-      <c r="E1982" s="54"/>
+      <c r="E1982" s="58"/>
     </row>
     <row r="1983" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1983" s="36"/>
@@ -26246,7 +26243,7 @@
       <c r="D1983" s="20">
         <v>5</v>
       </c>
-      <c r="E1983" s="53"/>
+      <c r="E1983" s="57"/>
     </row>
     <row r="1984" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1984" s="36"/>
@@ -26254,7 +26251,7 @@
       <c r="D1984" s="19">
         <v>6</v>
       </c>
-      <c r="E1984" s="52" t="s">
+      <c r="E1984" s="56" t="s">
         <v>1036</v>
       </c>
     </row>
@@ -26264,7 +26261,7 @@
       <c r="D1985" s="20">
         <v>7</v>
       </c>
-      <c r="E1985" s="53"/>
+      <c r="E1985" s="57"/>
     </row>
     <row r="1986" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1986" s="36"/>
@@ -26272,7 +26269,7 @@
       <c r="D1986" s="19">
         <v>8</v>
       </c>
-      <c r="E1986" s="52" t="s">
+      <c r="E1986" s="56" t="s">
         <v>1029</v>
       </c>
     </row>
@@ -26282,7 +26279,7 @@
       <c r="D1987" s="20">
         <v>9</v>
       </c>
-      <c r="E1987" s="53"/>
+      <c r="E1987" s="57"/>
     </row>
     <row r="1988" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1988" s="36"/>
@@ -26307,8 +26304,8 @@
       <c r="E1989" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="F1989" s="60" t="s">
-        <v>1225</v>
+      <c r="F1989" s="55" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="1990" spans="2:6" x14ac:dyDescent="0.2">
@@ -26391,7 +26388,7 @@
       <c r="E1996" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F1996" s="59" t="s">
+      <c r="F1996" s="54" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -26614,7 +26611,7 @@
       <c r="E2016" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F2016" s="57" t="s">
+      <c r="F2016" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -27080,7 +27077,7 @@
       <c r="E2057" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F2057" s="57" t="s">
+      <c r="F2057" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -27401,7 +27398,7 @@
       <c r="E2087" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F2087" s="57" t="s">
+      <c r="F2087" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -28686,7 +28683,7 @@
       <c r="E2205" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F2205" s="57" t="s">
+      <c r="F2205" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -28743,7 +28740,7 @@
       <c r="E2210" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F2210" s="57" t="s">
+      <c r="F2210" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -28780,7 +28777,7 @@
       <c r="E2213" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F2213" s="57" t="s">
+      <c r="F2213" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -28847,7 +28844,7 @@
       <c r="E2219" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F2219" s="57" t="s">
+      <c r="F2219" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -29232,7 +29229,7 @@
       <c r="E2254" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="F2254" s="57" t="s">
+      <c r="F2254" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -29343,6 +29340,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004F7AABC398522B40A32DAEEC36E85685" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fcd56fbdc9ca50fa66f2b7c9cf7a93ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="246f02dd96380beb4f7cdcce14d77fd6">
     <xsd:element name="properties">
@@ -29391,15 +29397,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBE20A7-1A06-4982-8E6C-B0692E74AD85}">
   <ds:schemaRefs>
@@ -29415,6 +29412,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BABB9296-97A3-46A1-A889-43BF8783A394}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29427,12 +29432,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>